<commit_message>
opción de medrar a vip
</commit_message>
<xml_diff>
--- a/TAREAS.xlsx
+++ b/TAREAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/f_perezh_edu_uah_es/Documents/0_UNI/0_programas/PROG/PL2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{48B31374-707B-4DC9-BFB8-3DA46CE15A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E0E18BB-7FB5-4C54-A41B-951ACADA2EBF}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{48B31374-707B-4DC9-BFB8-3DA46CE15A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12608368-579A-4387-8DDC-51D8B211B2A5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{92C9341A-C18B-4DB8-8CFA-EE1E21D67F7D}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{92C9341A-C18B-4DB8-8CFA-EE1E21D67F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -250,6 +250,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -571,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DCD8C0-6A6D-4007-8403-BEB57AFC6059}">
   <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,8 +648,8 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>18</v>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F8" s="6">
         <v>45431</v>
@@ -687,8 +691,8 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>18</v>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F13" s="6">
         <v>45431</v>

</xml_diff>